<commit_message>
preparing physiological noise cleaning
</commit_message>
<xml_diff>
--- a/mc/latest_experiment/task_cond_pt2_3x3.xlsx
+++ b/mc/latest_experiment/task_cond_pt2_3x3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\behrenslab-fmrib\Documents\Psychopy\musicbox\experiment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xpsy1114/Documents/projects/multiple_clocks/multiple_clocks_repo/mc/latest_experiment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A989EA8A-2773-4DE7-975A-3A03F2E16726}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC82F748-E76D-CC4E-8CD1-7C0FD9807865}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4410" yWindow="-14820" windowWidth="22485" windowHeight="11475" xr2:uid="{429C41B6-8FE1-478D-BD9D-A7308FDB1539}"/>
+    <workbookView xWindow="0" yWindow="8420" windowWidth="22480" windowHeight="11480" xr2:uid="{429C41B6-8FE1-478D-BD9D-A7308FDB1539}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -133,7 +133,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -143,6 +143,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -160,13 +166,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -485,12 +494,12 @@
   <dimension ref="A1:R11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -546,7 +555,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -602,7 +611,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="3" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -615,10 +624,10 @@
       <c r="D3" s="2">
         <v>-0.28999999999999998</v>
       </c>
-      <c r="E3" s="2">
-        <v>-0.21</v>
-      </c>
-      <c r="F3" s="2">
+      <c r="E3" s="4">
+        <v>-0.21</v>
+      </c>
+      <c r="F3" s="4">
         <v>0.28999999999999998</v>
       </c>
       <c r="G3" s="2">
@@ -627,10 +636,10 @@
       <c r="H3" s="2">
         <v>-0.28999999999999998</v>
       </c>
-      <c r="I3" s="2">
-        <v>-0.21</v>
-      </c>
-      <c r="J3" s="2">
+      <c r="I3" s="4">
+        <v>-0.21</v>
+      </c>
+      <c r="J3" s="4">
         <v>0.28999999999999998</v>
       </c>
       <c r="K3" s="1">
@@ -658,7 +667,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="4" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -714,17 +723,17 @@
         <v>73</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="5" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="2">
-        <v>0</v>
-      </c>
-      <c r="D5" s="2">
+      <c r="C5" s="4">
+        <v>0</v>
+      </c>
+      <c r="D5" s="4">
         <v>0.28999999999999998</v>
       </c>
       <c r="E5" s="2">
@@ -733,10 +742,10 @@
       <c r="F5" s="2">
         <v>-0.28999999999999998</v>
       </c>
-      <c r="G5" s="2">
-        <v>0</v>
-      </c>
-      <c r="H5" s="2">
+      <c r="G5" s="4">
+        <v>0</v>
+      </c>
+      <c r="H5" s="4">
         <v>0.28999999999999998</v>
       </c>
       <c r="I5" s="2">
@@ -770,7 +779,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="6" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -826,7 +835,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="7" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -882,7 +891,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="8" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -938,7 +947,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="9" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -994,7 +1003,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="10" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1050,7 +1059,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="11" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1112,20 +1121,20 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="ed418b43-0a99-45a6-8c2a-de77aaa3b951" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="ed418b43-0a99-45a6-8c2a-de77aaa3b951" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1364,14 +1373,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F82107FE-D4A0-4B48-AB62-277998F00998}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{70FD8B70-A963-4792-939F-E98106DD28DB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -1384,6 +1385,14 @@
     <ds:schemaRef ds:uri="5e82e697-b980-44b1-8a92-63271da03dd5"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F82107FE-D4A0-4B48-AB62-277998F00998}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>